<commit_message>
Commit for change in master subject
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMasters.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMasters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="15255" windowHeight="7185" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="15255" windowHeight="7185" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ExamMasterCategory_FormData" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>MasterCategoryName</t>
   </si>
@@ -72,9 +72,6 @@
     <t>BestOfSubject</t>
   </si>
   <si>
-    <t>Subject Group Without Elective</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>GENERAL SCIENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vaps Subject Group Without Elective</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,19 +619,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -644,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,19 +682,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -706,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -717,7 +720,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -725,7 +728,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>

</xml_diff>